<commit_message>
Actualización Datos y Creación Código Matlab
</commit_message>
<xml_diff>
--- a/Datos Municipios.xlsx
+++ b/Datos Municipios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PUJ\VIII Semestre\Planeación del Proyecto Final\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PUJ\VIII Semestre\Matlab - Herramienta Tecnológica\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A7B6C3-AD53-4C62-8E07-22C88DC35C2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A884BF-26E3-4A32-8533-78037E4AED74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3237,9 +3237,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -3265,6 +3265,11 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3286,7 +3291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3312,13 +3317,16 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3637,20 +3645,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B804" workbookViewId="0">
+      <selection activeCell="H824" sqref="H824"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -3662,10 +3670,10 @@
         <v>1035</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>1064</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>1065</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>1066</v>
@@ -3674,10 +3682,10 @@
         <v>1067</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>1069</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>1068</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>1069</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -3725,6 +3733,12 @@
       <c r="F3" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="G3" s="11">
+        <v>-1.9983070000000001</v>
+      </c>
+      <c r="H3" s="11">
+        <v>-72.692187000000004</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="7">
@@ -3745,6 +3759,12 @@
       <c r="F4" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="G4" s="11">
+        <v>-1.282386</v>
+      </c>
+      <c r="H4" s="11">
+        <v>-72.637698</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="7">
@@ -3765,6 +3785,12 @@
       <c r="F5" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="G5" s="11">
+        <v>-1.1950970000000001</v>
+      </c>
+      <c r="H5" s="11">
+        <v>-70.088775999999996</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="7">
@@ -3785,6 +3811,12 @@
       <c r="F6" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="G6" s="11">
+        <v>-0.121379</v>
+      </c>
+      <c r="H6" s="11">
+        <v>-71.082607999999993</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="7">
@@ -3805,6 +3837,12 @@
       <c r="F7" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="G7" s="11">
+        <v>-0.60822500000000002</v>
+      </c>
+      <c r="H7" s="11">
+        <v>-71.246443999999997</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="7">
@@ -3825,6 +3863,12 @@
       <c r="F8" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="G8" s="11">
+        <v>-0.95018100000000005</v>
+      </c>
+      <c r="H8" s="11">
+        <v>-73.841302999999996</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="7">
@@ -3845,6 +3889,12 @@
       <c r="F9" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="G9" s="11">
+        <v>-1.9591510000000001</v>
+      </c>
+      <c r="H9" s="11">
+        <v>-71.245524000000003</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="7">
@@ -3891,6 +3941,12 @@
       <c r="F11" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="G11" s="11">
+        <v>-1.078333</v>
+      </c>
+      <c r="H11" s="11">
+        <v>-72.184332999999995</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="7">
@@ -3911,6 +3967,12 @@
       <c r="F12" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="G12" s="11">
+        <v>-2.6100089999999998</v>
+      </c>
+      <c r="H12" s="11">
+        <v>-69.934121000000005</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="7">
@@ -7493,6 +7555,12 @@
       <c r="F150" s="5" t="s">
         <v>148</v>
       </c>
+      <c r="G150" s="11">
+        <v>10.826108</v>
+      </c>
+      <c r="H150" s="11">
+        <v>-75.086755999999994</v>
+      </c>
     </row>
     <row r="151" spans="1:8">
       <c r="A151" s="7">
@@ -10945,6 +11013,12 @@
       <c r="F283" s="5" t="s">
         <v>276</v>
       </c>
+      <c r="G283" s="11">
+        <v>5.6529249999999998</v>
+      </c>
+      <c r="H283" s="11">
+        <v>-72.375921000000005</v>
+      </c>
     </row>
     <row r="284" spans="1:8">
       <c r="A284" s="7">
@@ -13383,6 +13457,12 @@
       <c r="F377" s="5" t="s">
         <v>370</v>
       </c>
+      <c r="G377" s="11">
+        <v>0.240758</v>
+      </c>
+      <c r="H377" s="11">
+        <v>-72.521698000000001</v>
+      </c>
     </row>
     <row r="378" spans="1:8">
       <c r="A378" s="7">
@@ -16029,6 +16109,12 @@
       <c r="F479" s="5" t="s">
         <v>462</v>
       </c>
+      <c r="G479" s="11">
+        <v>5.8389069999999998</v>
+      </c>
+      <c r="H479" s="11">
+        <v>-76.207970000000003</v>
+      </c>
     </row>
     <row r="480" spans="1:8">
       <c r="A480" s="7">
@@ -16153,6 +16239,12 @@
       <c r="F484" s="5" t="s">
         <v>467</v>
       </c>
+      <c r="G484" s="11">
+        <v>5.9948860000000002</v>
+      </c>
+      <c r="H484" s="11">
+        <v>-76.782272000000006</v>
+      </c>
     </row>
     <row r="485" spans="1:8">
       <c r="A485" s="7">
@@ -16173,6 +16265,12 @@
       <c r="F485" s="5" t="s">
         <v>468</v>
       </c>
+      <c r="G485" s="11">
+        <v>5.1494650000000002</v>
+      </c>
+      <c r="H485" s="11">
+        <v>-76.986872000000005</v>
+      </c>
     </row>
     <row r="486" spans="1:8">
       <c r="A486" s="7">
@@ -16713,6 +16811,12 @@
       <c r="F506" s="5" t="s">
         <v>487</v>
       </c>
+      <c r="G506" s="11">
+        <v>8.0411000000000001</v>
+      </c>
+      <c r="H506" s="11">
+        <v>-75.313632999999996</v>
+      </c>
     </row>
     <row r="507" spans="1:8">
       <c r="A507" s="7">
@@ -20243,6 +20347,12 @@
       <c r="F642" s="5" t="s">
         <v>616</v>
       </c>
+      <c r="G642" s="11">
+        <v>4.7528220000000001</v>
+      </c>
+      <c r="H642" s="11">
+        <v>-74.379053999999996</v>
+      </c>
     </row>
     <row r="643" spans="1:8">
       <c r="A643" s="7">
@@ -20312,8 +20422,14 @@
       <c r="E645" s="7">
         <v>94343</v>
       </c>
-      <c r="F645" s="5" t="s">
+      <c r="F645" s="12" t="s">
         <v>619</v>
+      </c>
+      <c r="G645" s="11">
+        <v>3.49424</v>
+      </c>
+      <c r="H645" s="11">
+        <v>-69.813260999999997</v>
       </c>
     </row>
     <row r="646" spans="1:8">
@@ -20335,6 +20451,12 @@
       <c r="F646" s="5" t="s">
         <v>620</v>
       </c>
+      <c r="G646" s="11">
+        <v>2.8061449999999999</v>
+      </c>
+      <c r="H646" s="11">
+        <v>-70.477999999999994</v>
+      </c>
     </row>
     <row r="647" spans="1:8">
       <c r="A647" s="7">
@@ -20355,6 +20477,12 @@
       <c r="F647" s="5" t="s">
         <v>621</v>
       </c>
+      <c r="G647" s="11">
+        <v>1.9136770000000001</v>
+      </c>
+      <c r="H647" s="11">
+        <v>-67.067550999999995</v>
+      </c>
     </row>
     <row r="648" spans="1:8">
       <c r="A648" s="7">
@@ -20375,6 +20503,12 @@
       <c r="F648" s="5" t="s">
         <v>156</v>
       </c>
+      <c r="G648" s="11">
+        <v>2.4954969999999999</v>
+      </c>
+      <c r="H648" s="11">
+        <v>-68.270510999999999</v>
+      </c>
     </row>
     <row r="649" spans="1:8">
       <c r="A649" s="7">
@@ -20395,6 +20529,12 @@
       <c r="F649" s="5" t="s">
         <v>622</v>
       </c>
+      <c r="G649" s="11">
+        <v>1.418903</v>
+      </c>
+      <c r="H649" s="11">
+        <v>-66.997681999999998</v>
+      </c>
     </row>
     <row r="650" spans="1:8">
       <c r="A650" s="7">
@@ -20415,6 +20555,12 @@
       <c r="F650" s="5" t="s">
         <v>623</v>
       </c>
+      <c r="G650" s="11">
+        <v>3.5261710000000002</v>
+      </c>
+      <c r="H650" s="11">
+        <v>-67.412542000000002</v>
+      </c>
     </row>
     <row r="651" spans="1:8">
       <c r="A651" s="7">
@@ -20435,6 +20581,12 @@
       <c r="F651" s="5" t="s">
         <v>624</v>
       </c>
+      <c r="G651" s="11">
+        <v>2.0633720000000002</v>
+      </c>
+      <c r="H651" s="11">
+        <v>-69.084846999999996</v>
+      </c>
     </row>
     <row r="652" spans="1:8">
       <c r="A652" s="7">
@@ -20455,6 +20607,12 @@
       <c r="F652" s="5" t="s">
         <v>625</v>
       </c>
+      <c r="G652" s="11">
+        <v>2.4160140000000001</v>
+      </c>
+      <c r="H652" s="11">
+        <v>-69.910641999999996</v>
+      </c>
     </row>
     <row r="653" spans="1:8">
       <c r="A653" s="7">
@@ -22295,6 +22453,12 @@
       <c r="F723" s="5" t="s">
         <v>687</v>
       </c>
+      <c r="G723" s="11">
+        <v>10.149076000000001</v>
+      </c>
+      <c r="H723" s="11">
+        <v>-74.837766000000002</v>
+      </c>
     </row>
     <row r="724" spans="1:8">
       <c r="A724" s="7">
@@ -22679,6 +22843,12 @@
       <c r="F738" s="5" t="s">
         <v>701</v>
       </c>
+      <c r="G738" s="11">
+        <v>10.796920999999999</v>
+      </c>
+      <c r="H738" s="11">
+        <v>-74.180778000000004</v>
+      </c>
     </row>
     <row r="739" spans="1:8">
       <c r="A739" s="7">
@@ -23947,6 +24117,12 @@
       <c r="F787" s="5" t="s">
         <v>743</v>
       </c>
+      <c r="G787" s="11">
+        <v>1.394995</v>
+      </c>
+      <c r="H787" s="11">
+        <v>76.992564000000002</v>
+      </c>
     </row>
     <row r="788" spans="1:8">
       <c r="A788" s="7">
@@ -24903,6 +25079,12 @@
       <c r="F824" s="5" t="s">
         <v>111</v>
       </c>
+      <c r="G824" s="11">
+        <v>1.28016</v>
+      </c>
+      <c r="H824" s="11">
+        <v>-77.419169999999994</v>
+      </c>
     </row>
     <row r="825" spans="1:8">
       <c r="A825" s="7">
@@ -27159,6 +27341,12 @@
       <c r="F911" s="5" t="s">
         <v>847</v>
       </c>
+      <c r="G911" s="11">
+        <v>12.588684000000001</v>
+      </c>
+      <c r="H911" s="11">
+        <v>-81.700204999999997</v>
+      </c>
     </row>
     <row r="912" spans="1:8">
       <c r="A912" s="7">
@@ -28115,6 +28303,12 @@
       <c r="F948" s="5" t="s">
         <v>876</v>
       </c>
+      <c r="G948" s="11">
+        <v>7.0732330000000001</v>
+      </c>
+      <c r="H948" s="11">
+        <v>-73.16892</v>
+      </c>
     </row>
     <row r="949" spans="1:8">
       <c r="A949" s="7">
@@ -30111,6 +30305,12 @@
       <c r="F1025" s="5" t="s">
         <v>942</v>
       </c>
+      <c r="G1025" s="11">
+        <v>9.4495229999999992</v>
+      </c>
+      <c r="H1025" s="11">
+        <v>-75.431274000000002</v>
+      </c>
     </row>
     <row r="1026" spans="1:8">
       <c r="A1026" s="7">
@@ -31925,6 +32125,12 @@
       <c r="F1095" s="5" t="s">
         <v>1007</v>
       </c>
+      <c r="G1095" s="11">
+        <v>3.6962999999999999</v>
+      </c>
+      <c r="H1095" s="11">
+        <v>-76.578481999999994</v>
+      </c>
     </row>
     <row r="1096" spans="1:8">
       <c r="A1096" s="7">
@@ -32491,6 +32697,12 @@
       <c r="F1117" s="5" t="s">
         <v>1025</v>
       </c>
+      <c r="G1117" s="11">
+        <v>0.19420200000000001</v>
+      </c>
+      <c r="H1117" s="11">
+        <v>-70.907458000000005</v>
+      </c>
     </row>
     <row r="1118" spans="1:8">
       <c r="A1118" s="7">
@@ -32537,6 +32749,12 @@
       <c r="F1119" s="5" t="s">
         <v>1027</v>
       </c>
+      <c r="G1119" s="11">
+        <v>1.912817</v>
+      </c>
+      <c r="H1119" s="11">
+        <v>-70.608354000000006</v>
+      </c>
     </row>
     <row r="1120" spans="1:8">
       <c r="A1120" s="7">
@@ -32556,6 +32774,12 @@
       </c>
       <c r="F1120" s="5" t="s">
         <v>1028</v>
+      </c>
+      <c r="G1120" s="11">
+        <v>0.83142099999999997</v>
+      </c>
+      <c r="H1120" s="11">
+        <v>-69.634243999999995</v>
       </c>
     </row>
     <row r="1121" spans="1:8">

</xml_diff>